<commit_message>
Day-2, doing string questions of love-babber sheet, lcs, longest repeating subseq...
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01203629-E1BD-4139-82EC-B8E82E463F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB51FDC-90F0-4CF1-BA38-A234C3D72FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="470">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1869,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B56" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="C56" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2535,9 +2535,7 @@
       <c r="B63" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="C63" s="4"/>
       <c r="D63" t="s">
         <v>469</v>
       </c>

</xml_diff>

<commit_message>
Day-7, doing rabincarp or lcs related queestions
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB51FDC-90F0-4CF1-BA38-A234C3D72FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19735B-561E-4959-9F15-266259FEB844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="471">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1435,6 +1435,9 @@
   </si>
   <si>
     <t xml:space="preserve">                Done</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1869,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C56" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2564,9 +2567,6 @@
       <c r="C65" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="D65" t="s">
-        <v>469</v>
-      </c>
     </row>
     <row r="66" spans="1:4" ht="21">
       <c r="A66" s="5" t="s">
@@ -2575,11 +2575,9 @@
       <c r="B66" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="C66" s="4"/>
       <c r="D66" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="21">
@@ -2589,11 +2587,9 @@
       <c r="B67" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="C67" s="4"/>
       <c r="D67" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="21">
@@ -2606,9 +2602,6 @@
       <c r="C68" s="4" t="s">
         <v>466</v>
       </c>
-      <c r="D68" t="s">
-        <v>469</v>
-      </c>
     </row>
     <row r="69" spans="1:4" ht="21">
       <c r="A69" s="5" t="s">
@@ -2617,11 +2610,9 @@
       <c r="B69" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="4" t="s">
-        <v>466</v>
-      </c>
+      <c r="C69" s="4"/>
       <c r="D69" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="21">
@@ -2631,8 +2622,9 @@
       <c r="B70" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="4" t="s">
-        <v>466</v>
+      <c r="C70" s="4"/>
+      <c r="D70" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="21">
@@ -2642,8 +2634,9 @@
       <c r="B71" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="4" t="s">
-        <v>466</v>
+      <c r="C71" s="4"/>
+      <c r="D71" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="21">
@@ -2664,8 +2657,9 @@
       <c r="B73" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C73" s="4" t="s">
-        <v>466</v>
+      <c r="C73" s="4"/>
+      <c r="D73" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Day-8, start to do tree questions series
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C19735B-561E-4959-9F15-266259FEB844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1A364-4E26-4975-BFB8-0A3E116D50D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3255,7 +3255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="21">
+    <row r="129" spans="1:4" ht="21">
       <c r="A129" s="5" t="s">
         <v>97</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="21">
+    <row r="130" spans="1:4" ht="21">
       <c r="A130" s="5" t="s">
         <v>97</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="21">
+    <row r="131" spans="1:4" ht="21">
       <c r="A131" s="5" t="s">
         <v>97</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="21">
+    <row r="132" spans="1:4" ht="21">
       <c r="A132" s="5" t="s">
         <v>97</v>
       </c>
@@ -3299,7 +3299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="21">
+    <row r="133" spans="1:4" ht="21">
       <c r="A133" s="5" t="s">
         <v>97</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="21">
+    <row r="134" spans="1:4" ht="21">
       <c r="A134" s="5" t="s">
         <v>97</v>
       </c>
@@ -3321,7 +3321,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="21">
+    <row r="135" spans="1:4" ht="21">
       <c r="A135" s="5" t="s">
         <v>97</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="21">
+    <row r="136" spans="1:4" ht="21">
       <c r="A136" s="5" t="s">
         <v>97</v>
       </c>
@@ -3343,22 +3343,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="21">
+    <row r="138" spans="1:4" ht="21">
       <c r="B138" s="7"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" ht="21">
+    <row r="139" spans="1:4" ht="21">
       <c r="A139" s="8" t="s">
         <v>134</v>
       </c>
       <c r="B139" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C139" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="21">
+      <c r="C139" s="4"/>
+      <c r="D139" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="21">
       <c r="A140" s="8" t="s">
         <v>134</v>
       </c>
@@ -3369,7 +3370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="21">
+    <row r="141" spans="1:4" ht="21">
       <c r="A141" s="8" t="s">
         <v>134</v>
       </c>
@@ -3380,7 +3381,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="21">
+    <row r="142" spans="1:4" ht="21">
       <c r="A142" s="8" t="s">
         <v>134</v>
       </c>
@@ -3391,7 +3392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="21">
+    <row r="143" spans="1:4" ht="21">
       <c r="A143" s="8" t="s">
         <v>134</v>
       </c>
@@ -3402,7 +3403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="21">
+    <row r="144" spans="1:4" ht="21">
       <c r="A144" s="8" t="s">
         <v>134</v>
       </c>
@@ -3755,7 +3756,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3766,7 +3767,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3777,7 +3778,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">

</xml_diff>

<commit_message>
D-9,Doing tree question dimeter, and mirror node, Day-2
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1A364-4E26-4975-BFB8-0A3E116D50D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17EEB3A-8066-47C5-B7BE-3923D7FCBB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3789,7 +3789,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3800,7 +3800,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-10, Doing tree traversal types of questions, LNR, NLR, LRN, Day-3
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17EEB3A-8066-47C5-B7BE-3923D7FCBB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA386C-E713-45D9-B3D2-CD097CE15633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
-      <selection activeCell="B182" sqref="B182"/>
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3811,7 +3811,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3822,7 +3822,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3833,7 +3833,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-11, Doing tree traverse/views questions, Day-4
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CA386C-E713-45D9-B3D2-CD097CE15633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B9379-0C8F-4CD5-82AA-A01FB30B4EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B172" workbookViewId="0">
-      <selection activeCell="B185" sqref="B185"/>
+    <sheetView tabSelected="1" topLeftCell="B180" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3844,7 +3844,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3855,7 +3855,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3866,7 +3866,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3877,7 +3877,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3888,7 +3888,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-12, Doing tree trversal and check balance tree questions, D-5
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0B9379-0C8F-4CD5-82AA-A01FB30B4EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B49065-DA29-4970-8524-CB38253999D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1873,7 +1873,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B180" workbookViewId="0">
-      <selection activeCell="B190" sqref="B190"/>
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3899,7 +3899,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3910,7 +3910,7 @@
         <v>186</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-13, try to end tree series, D-6
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B49065-DA29-4970-8524-CB38253999D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D1D1F1-C0E0-4F60-A2CB-9EBCD9F0FF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1872,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B180" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+    <sheetView tabSelected="1" topLeftCell="B200" workbookViewId="0">
+      <selection activeCell="B209" sqref="B209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3921,7 +3921,7 @@
         <v>187</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">
@@ -4086,7 +4086,7 @@
         <v>202</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="208" spans="1:3" ht="21">
@@ -4097,7 +4097,7 @@
         <v>203</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="209" spans="1:3" ht="21">
@@ -4119,7 +4119,7 @@
         <v>205</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="211" spans="1:3" ht="21">
@@ -4130,7 +4130,7 @@
         <v>206</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-14, Doing tree questions D-7
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D1D1F1-C0E0-4F60-A2CB-9EBCD9F0FF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD5BDA-1170-481F-9E30-8F0A40D0EED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1358" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="473">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1438,13 +1438,19 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Repeat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1506,13 +1512,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1524,11 +1554,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1555,9 +1587,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1872,8 +1913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B200" workbookViewId="0">
-      <selection activeCell="B209" sqref="B209"/>
+    <sheetView tabSelected="1" topLeftCell="B192" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3924,7 +3965,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="21">
+    <row r="193" spans="1:4" ht="21">
       <c r="A193" s="5" t="s">
         <v>171</v>
       </c>
@@ -3932,10 +3973,10 @@
         <v>188</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="21">
       <c r="A194" s="5" t="s">
         <v>171</v>
       </c>
@@ -3946,7 +3987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="21">
+    <row r="195" spans="1:4" ht="21">
       <c r="A195" s="5" t="s">
         <v>171</v>
       </c>
@@ -3954,10 +3995,10 @@
         <v>190</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="196" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="21">
       <c r="A196" s="5" t="s">
         <v>171</v>
       </c>
@@ -3965,10 +4006,10 @@
         <v>191</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="21">
       <c r="A197" s="5" t="s">
         <v>171</v>
       </c>
@@ -3979,7 +4020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:3" ht="21">
+    <row r="198" spans="1:4" ht="21">
       <c r="A198" s="5" t="s">
         <v>171</v>
       </c>
@@ -3990,7 +4031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="21">
+    <row r="199" spans="1:4" ht="21">
       <c r="A199" s="5" t="s">
         <v>171</v>
       </c>
@@ -4001,7 +4042,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="21">
+    <row r="200" spans="1:4" ht="21">
       <c r="A200" s="5" t="s">
         <v>171</v>
       </c>
@@ -4012,91 +4053,97 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="21">
+    <row r="201" spans="1:4" ht="21">
       <c r="A201" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B201" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="C201" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="21">
+      <c r="C201" s="14" t="s">
+        <v>470</v>
+      </c>
+      <c r="D201" s="13" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="21">
       <c r="A202" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B202" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C202" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="21">
+      <c r="C202" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="21">
       <c r="A203" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B203" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="C203" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3" ht="21">
+      <c r="C203" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D203" s="13" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="21">
       <c r="A204" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B204" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="C204" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="205" spans="1:3" ht="21">
+      <c r="C204" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="21">
       <c r="A205" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B205" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C205" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3" ht="21">
+      <c r="C205" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="21">
       <c r="A206" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B206" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="C206" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" ht="21">
+      <c r="C206" s="12" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="21">
       <c r="A207" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B207" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="C207" s="4" t="s">
+      <c r="C207" s="12" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="208" spans="1:3" ht="21">
+    <row r="208" spans="1:4" ht="21">
       <c r="A208" s="5" t="s">
         <v>171</v>
       </c>
       <c r="B208" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C208" s="4" t="s">
+      <c r="C208" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4107,8 +4154,8 @@
       <c r="B209" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="C209" s="4" t="s">
-        <v>4</v>
+      <c r="C209" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="210" spans="1:3" ht="21">
@@ -4118,7 +4165,7 @@
       <c r="B210" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C210" s="4" t="s">
+      <c r="C210" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4129,7 +4176,7 @@
       <c r="B211" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="C211" s="4" t="s">
+      <c r="C211" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -6981,6 +7028,16 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C207">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="formula" val="&quot;Done&quot;"/>
+        <cfvo type="formula" val="&quot;Done&quot;"/>
+        <color theme="9"/>
+        <color theme="9"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{9492A4AD-FA44-BA4B-B154-E4DBB1951162}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{2D6F1134-3C08-7445-B19A-9B94A18B55C7}"/>

</xml_diff>

<commit_message>
Day-15, Completing the tree series, now we are on the BST series... ➡️
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3CD5BDA-1170-481F-9E30-8F0A40D0EED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40259727-9477-46EE-AFE1-D1DE840F3727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1360" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="474">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1444,6 +1444,9 @@
   </si>
   <si>
     <t xml:space="preserve">                  Repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                Repeat</t>
   </si>
 </sst>
 </file>
@@ -1914,7 +1917,7 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B192" workbookViewId="0">
-      <selection activeCell="B199" sqref="B199"/>
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3983,8 +3986,11 @@
       <c r="B194" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="C194" s="4" t="s">
-        <v>4</v>
+      <c r="C194" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D194" s="13" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="195" spans="1:4" ht="21">
@@ -4039,7 +4045,7 @@
         <v>194</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="200" spans="1:4" ht="21">
@@ -4050,7 +4056,7 @@
         <v>195</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="201" spans="1:4" ht="21">

</xml_diff>

<commit_message>
Day-16/17, Completed BST sheet question, too easy in compare of I think.., now doing youtube question of love babber
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40259727-9477-46EE-AFE1-D1DE840F3727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7138B-8F92-4312-93E1-7AACCB39A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B192" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" topLeftCell="B223" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4203,8 +4203,8 @@
       <c r="B214" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="C214" s="4" t="s">
-        <v>4</v>
+      <c r="C214" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4214,8 +4214,8 @@
       <c r="B215" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="C215" s="4" t="s">
-        <v>4</v>
+      <c r="C215" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="216" spans="1:3" ht="21">
@@ -4225,8 +4225,8 @@
       <c r="B216" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="C216" s="4" t="s">
-        <v>4</v>
+      <c r="C216" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4236,8 +4236,8 @@
       <c r="B217" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="C217" s="4" t="s">
-        <v>4</v>
+      <c r="C217" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="218" spans="1:3" ht="21">
@@ -4247,8 +4247,8 @@
       <c r="B218" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="C218" s="4" t="s">
-        <v>4</v>
+      <c r="C218" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4269,8 +4269,8 @@
       <c r="B220" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C220" s="4" t="s">
-        <v>4</v>
+      <c r="C220" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="221" spans="1:3" ht="21">
@@ -4280,8 +4280,8 @@
       <c r="B221" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="C221" s="4" t="s">
-        <v>4</v>
+      <c r="C221" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="222" spans="1:3" ht="21">
@@ -4291,8 +4291,8 @@
       <c r="B222" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>4</v>
+      <c r="C222" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="223" spans="1:3" ht="21">
@@ -4303,7 +4303,7 @@
         <v>217</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="224" spans="1:3" ht="21">
@@ -4314,7 +4314,7 @@
         <v>218</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="225" spans="1:3" ht="21">
@@ -4325,7 +4325,7 @@
         <v>219</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="21">
@@ -4336,7 +4336,7 @@
         <v>220</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="21">
@@ -4347,7 +4347,7 @@
         <v>221</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="228" spans="1:3" ht="21">
@@ -4358,7 +4358,7 @@
         <v>222</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="21">
@@ -4369,7 +4369,7 @@
         <v>223</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="21">
@@ -4380,7 +4380,7 @@
         <v>224</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="231" spans="1:3" ht="21">
@@ -4391,7 +4391,7 @@
         <v>225</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="232" spans="1:3" ht="21">
@@ -4402,7 +4402,7 @@
         <v>226</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="21">
@@ -4413,7 +4413,7 @@
         <v>227</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="234" spans="1:3" ht="21">
@@ -4435,7 +4435,7 @@
         <v>229</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-18,Start to do heap series questions...
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F7138B-8F92-4312-93E1-7AACCB39A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36585833-2153-4FD0-B32F-5D8B116C35FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B223" workbookViewId="0">
-      <selection activeCell="B231" sqref="B231"/>
+    <sheetView tabSelected="1" topLeftCell="B330" workbookViewId="0">
+      <selection activeCell="C335" sqref="C335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4424,7 +4424,7 @@
         <v>228</v>
       </c>
       <c r="C234" s="4" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-19, Doing heap questions,maximum subarray ele, kth largest and smallest
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36585833-2153-4FD0-B32F-5D8B116C35FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E84999-1BD9-42CB-AD3C-98CE2D9BFA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -1916,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B330" workbookViewId="0">
-      <selection activeCell="C335" sqref="C335"/>
+    <sheetView tabSelected="1" topLeftCell="B334" workbookViewId="0">
+      <selection activeCell="C338" sqref="C338:C341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4302,7 +4302,7 @@
       <c r="B223" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="C223" s="4" t="s">
+      <c r="C223" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4313,7 +4313,7 @@
       <c r="B224" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="C224" s="4" t="s">
+      <c r="C224" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4324,7 +4324,7 @@
       <c r="B225" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="C225" s="4" t="s">
+      <c r="C225" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4335,7 +4335,7 @@
       <c r="B226" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="C226" s="4" t="s">
+      <c r="C226" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4346,7 +4346,7 @@
       <c r="B227" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="C227" s="4" t="s">
+      <c r="C227" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4357,7 +4357,7 @@
       <c r="B228" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="C228" s="4" t="s">
+      <c r="C228" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4368,7 +4368,7 @@
       <c r="B229" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="C229" s="4" t="s">
+      <c r="C229" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4379,7 +4379,7 @@
       <c r="B230" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="C230" s="4" t="s">
+      <c r="C230" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4390,7 +4390,7 @@
       <c r="B231" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="C231" s="4" t="s">
+      <c r="C231" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4401,7 +4401,7 @@
       <c r="B232" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="C232" s="4" t="s">
+      <c r="C232" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4412,7 +4412,7 @@
       <c r="B233" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="C233" s="4" t="s">
+      <c r="C233" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4423,7 +4423,7 @@
       <c r="B234" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="C234" s="4" t="s">
+      <c r="C234" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -4434,7 +4434,7 @@
       <c r="B235" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="C235" s="4" t="s">
+      <c r="C235" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5489,8 +5489,8 @@
       <c r="B336" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="C336" s="4" t="s">
-        <v>4</v>
+      <c r="C336" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="21">
@@ -5500,8 +5500,8 @@
       <c r="B337" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C337" s="4" t="s">
-        <v>4</v>
+      <c r="C337" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="21">
@@ -5511,8 +5511,8 @@
       <c r="B338" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="C338" s="4" t="s">
-        <v>4</v>
+      <c r="C338" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5522,8 +5522,8 @@
       <c r="B339" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="C339" s="4" t="s">
-        <v>4</v>
+      <c r="C339" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="21">
@@ -5533,8 +5533,8 @@
       <c r="B340" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C340" s="4" t="s">
-        <v>4</v>
+      <c r="C340" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="341" spans="1:3" ht="21">
@@ -5544,8 +5544,8 @@
       <c r="B341" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="C341" s="4" t="s">
-        <v>4</v>
+      <c r="C341" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Day-20, Mostly merging in a vector questions
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E84999-1BD9-42CB-AD3C-98CE2D9BFA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A854C4-86F1-423C-83C0-7475F9C2E08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="475">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1447,6 +1447,9 @@
   </si>
   <si>
     <t xml:space="preserve">                Repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Repeat</t>
   </si>
 </sst>
 </file>
@@ -1916,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:D481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B334" workbookViewId="0">
-      <selection activeCell="C338" sqref="C338:C341"/>
+    <sheetView tabSelected="1" topLeftCell="B341" workbookViewId="0">
+      <selection activeCell="B348" sqref="B348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5493,7 +5496,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="337" spans="1:3" ht="21">
+    <row r="337" spans="1:4" ht="21">
       <c r="A337" s="8" t="s">
         <v>324</v>
       </c>
@@ -5504,7 +5507,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="338" spans="1:3" ht="21">
+    <row r="338" spans="1:4" ht="21">
       <c r="A338" s="8" t="s">
         <v>324</v>
       </c>
@@ -5515,7 +5518,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="339" spans="1:3" ht="21">
+    <row r="339" spans="1:4" ht="21">
       <c r="A339" s="8" t="s">
         <v>324</v>
       </c>
@@ -5526,7 +5529,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="340" spans="1:3" ht="21">
+    <row r="340" spans="1:4" ht="21">
       <c r="A340" s="8" t="s">
         <v>324</v>
       </c>
@@ -5537,7 +5540,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="341" spans="1:3" ht="21">
+    <row r="341" spans="1:4" ht="21">
       <c r="A341" s="8" t="s">
         <v>324</v>
       </c>
@@ -5548,7 +5551,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="342" spans="1:3" ht="21">
+    <row r="342" spans="1:4" ht="21">
       <c r="A342" s="8" t="s">
         <v>324</v>
       </c>
@@ -5556,10 +5559,10 @@
         <v>331</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="343" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" ht="21">
       <c r="A343" s="8" t="s">
         <v>324</v>
       </c>
@@ -5567,10 +5570,10 @@
         <v>332</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="344" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" ht="21">
       <c r="A344" s="8" t="s">
         <v>324</v>
       </c>
@@ -5578,10 +5581,10 @@
         <v>333</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="345" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" ht="21">
       <c r="A345" s="8" t="s">
         <v>324</v>
       </c>
@@ -5589,32 +5592,38 @@
         <v>334</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="346" spans="1:3" ht="21">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" ht="21">
       <c r="A346" s="8" t="s">
         <v>324</v>
       </c>
       <c r="B346" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="C346" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="347" spans="1:3" ht="21">
+      <c r="C346" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D346" s="13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" ht="21">
       <c r="A347" s="8" t="s">
         <v>324</v>
       </c>
       <c r="B347" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C347" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="348" spans="1:3" ht="21">
+      <c r="C347" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D347" s="13" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" ht="21">
       <c r="A348" s="8" t="s">
         <v>324</v>
       </c>
@@ -5625,7 +5634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:3" ht="21">
+    <row r="349" spans="1:4" ht="21">
       <c r="A349" s="8" t="s">
         <v>324</v>
       </c>
@@ -5636,7 +5645,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:3" ht="21">
+    <row r="350" spans="1:4" ht="21">
       <c r="A350" s="8" t="s">
         <v>324</v>
       </c>
@@ -5647,7 +5656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:3" ht="21">
+    <row r="351" spans="1:4" ht="21">
       <c r="A351" s="8" t="s">
         <v>324</v>
       </c>
@@ -5658,7 +5667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:3" ht="21">
+    <row r="352" spans="1:4" ht="21">
       <c r="A352" s="8" t="s">
         <v>324</v>
       </c>

</xml_diff>

<commit_message>
Day-23, I skip day-21,and 22 because of busy, now completed my heap series, move on graph series...
</commit_message>
<xml_diff>
--- a/Love-babber.xlsx
+++ b/Love-babber.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\10_SHEETS_SOLUTIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A854C4-86F1-423C-83C0-7475F9C2E08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B8344E-B2E6-4B65-A4C2-045EAB4A01F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -5558,7 +5558,7 @@
       <c r="B342" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="C342" s="4" t="s">
+      <c r="C342" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5569,7 +5569,7 @@
       <c r="B343" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C343" s="4" t="s">
+      <c r="C343" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5580,7 +5580,7 @@
       <c r="B344" s="9" t="s">
         <v>333</v>
       </c>
-      <c r="C344" s="4" t="s">
+      <c r="C344" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5591,7 +5591,7 @@
       <c r="B345" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C345" s="4" t="s">
+      <c r="C345" s="12" t="s">
         <v>470</v>
       </c>
     </row>
@@ -5603,7 +5603,7 @@
         <v>335</v>
       </c>
       <c r="C346" s="14" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
       <c r="D346" s="13" t="s">
         <v>474</v>
@@ -5617,7 +5617,7 @@
         <v>336</v>
       </c>
       <c r="C347" s="14" t="s">
-        <v>4</v>
+        <v>470</v>
       </c>
       <c r="D347" s="13" t="s">
         <v>474</v>
@@ -5630,8 +5630,8 @@
       <c r="B348" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="C348" s="4" t="s">
-        <v>4</v>
+      <c r="C348" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="349" spans="1:4" ht="21">
@@ -5641,8 +5641,8 @@
       <c r="B349" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="C349" s="4" t="s">
-        <v>4</v>
+      <c r="C349" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="350" spans="1:4" ht="21">
@@ -5652,8 +5652,8 @@
       <c r="B350" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C350" s="4" t="s">
-        <v>4</v>
+      <c r="C350" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="351" spans="1:4" ht="21">
@@ -5663,8 +5663,8 @@
       <c r="B351" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="C351" s="4" t="s">
-        <v>4</v>
+      <c r="C351" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="352" spans="1:4" ht="21">
@@ -5674,8 +5674,8 @@
       <c r="B352" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C352" s="4" t="s">
-        <v>4</v>
+      <c r="C352" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="21">
@@ -5685,8 +5685,8 @@
       <c r="B353" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C353" s="4" t="s">
-        <v>4</v>
+      <c r="C353" s="12" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="21">

</xml_diff>